<commit_message>
average over return periods works well with single and multi hazard data
</commit_message>
<xml_diff>
--- a/all_data_compiled.xlsx
+++ b/all_data_compiled.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>description</t>
   </si>
@@ -91,6 +91,9 @@
     <t>Elasticity of utility</t>
   </si>
   <si>
+    <t>Discount rate</t>
+  </si>
+  <si>
     <t>gdp_pc_pp</t>
   </si>
   <si>
@@ -160,7 +163,10 @@
     <t>income_elast</t>
   </si>
   <si>
-    <t>Province</t>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>province</t>
   </si>
   <si>
     <t>Abra</t>
@@ -758,13 +764,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X83"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,89 +843,95 @@
       <c r="X1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Y1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>133.688</v>
@@ -990,10 +1002,13 @@
       <c r="X4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>179.014</v>
@@ -1064,10 +1079,13 @@
       <c r="X5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Y5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>126.492</v>
@@ -1138,10 +1156,13 @@
       <c r="X6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Y6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>119.962</v>
@@ -1212,10 +1233,13 @@
       <c r="X7">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Y7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>158.629</v>
@@ -1286,10 +1310,13 @@
       <c r="X8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Y8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>124.667</v>
@@ -1360,10 +1387,13 @@
       <c r="X9">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="Y9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>158.732</v>
@@ -1434,10 +1464,13 @@
       <c r="X10">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="Y10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>175.235</v>
@@ -1508,10 +1541,13 @@
       <c r="X11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="Y11">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>134.8675</v>
@@ -1582,10 +1618,13 @@
       <c r="X12">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="Y12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>277.019</v>
@@ -1656,10 +1695,13 @@
       <c r="X13">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="Y13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>316.686</v>
@@ -1727,10 +1769,13 @@
       <c r="X14">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="Y14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>219.272</v>
@@ -1801,10 +1846,13 @@
       <c r="X15">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="Y15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B16">
         <v>303.525</v>
@@ -1875,10 +1923,13 @@
       <c r="X16">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:24">
+      <c r="Y16">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17">
         <v>237.761</v>
@@ -1949,10 +2000,13 @@
       <c r="X17">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:24">
+      <c r="Y17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>148.638</v>
@@ -2023,10 +2077,13 @@
       <c r="X18">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Y18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B19">
         <v>145.749</v>
@@ -2097,10 +2154,13 @@
       <c r="X19">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Y19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>253.279</v>
@@ -2171,10 +2231,13 @@
       <c r="X20">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:24">
+      <c r="Y20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B21">
         <v>179.424</v>
@@ -2245,10 +2308,13 @@
       <c r="X21">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:24">
+      <c r="Y21">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B22">
         <v>149.238</v>
@@ -2319,10 +2385,13 @@
       <c r="X22">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:24">
+      <c r="Y22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B23">
         <v>152.074</v>
@@ -2393,10 +2462,13 @@
       <c r="X23">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:24">
+      <c r="Y23">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B24">
         <v>156.261</v>
@@ -2467,10 +2539,13 @@
       <c r="X24">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="Y24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B25">
         <v>177.386</v>
@@ -2541,10 +2616,13 @@
       <c r="X25">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:24">
+      <c r="Y25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B26">
         <v>241.147</v>
@@ -2615,10 +2693,13 @@
       <c r="X26">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:24">
+      <c r="Y26">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B27">
         <v>282.606</v>
@@ -2689,10 +2770,13 @@
       <c r="X27">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:24">
+      <c r="Y27">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B28">
         <v>207.478</v>
@@ -2763,10 +2847,13 @@
       <c r="X28">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="Y28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B29">
         <v>137.747</v>
@@ -2837,10 +2924,13 @@
       <c r="X29">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:24">
+      <c r="Y29">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B30">
         <v>156.283</v>
@@ -2911,10 +3001,13 @@
       <c r="X30">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="Y30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B31">
         <v>190.398</v>
@@ -2985,10 +3078,13 @@
       <c r="X31">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="Y31">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32">
         <v>97.289</v>
@@ -3059,10 +3155,13 @@
       <c r="X32">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="Y32">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C33">
         <v>131195.356598692</v>
@@ -3118,10 +3217,13 @@
       <c r="X33">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:24">
+      <c r="Y33">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B34">
         <v>130.115</v>
@@ -3192,10 +3294,13 @@
       <c r="X34">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:24">
+      <c r="Y34">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B35">
         <v>162.895</v>
@@ -3266,10 +3371,13 @@
       <c r="X35">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:24">
+      <c r="Y35">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B36">
         <v>149.062</v>
@@ -3340,10 +3448,13 @@
       <c r="X36">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:24">
+      <c r="Y36">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B37">
         <v>192.382</v>
@@ -3414,10 +3525,13 @@
       <c r="X37">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:24">
+      <c r="Y37">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
       <c r="A38" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B38">
         <v>175.91</v>
@@ -3488,10 +3602,13 @@
       <c r="X38">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:24">
+      <c r="Y38">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B39">
         <v>187.023</v>
@@ -3562,10 +3679,13 @@
       <c r="X39">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:24">
+      <c r="Y39">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B40">
         <v>169.871</v>
@@ -3636,10 +3756,13 @@
       <c r="X40">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:24">
+      <c r="Y40">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B41">
         <v>170.385</v>
@@ -3710,10 +3833,13 @@
       <c r="X41">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:24">
+      <c r="Y41">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
       <c r="A42" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B42">
         <v>206.399</v>
@@ -3784,10 +3910,13 @@
       <c r="X42">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:24">
+      <c r="Y42">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
       <c r="A43" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B43">
         <v>249.092</v>
@@ -3858,10 +3987,13 @@
       <c r="X43">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:24">
+      <c r="Y43">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B44">
         <v>164.672</v>
@@ -3932,10 +4064,13 @@
       <c r="X44">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:24">
+      <c r="Y44">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
       <c r="A45" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B45">
         <v>131.981</v>
@@ -4006,10 +4141,13 @@
       <c r="X45">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:24">
+      <c r="Y45">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B46">
         <v>178.397</v>
@@ -4080,10 +4218,13 @@
       <c r="X46">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:24">
+      <c r="Y46">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
       <c r="A47" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B47">
         <v>140.218</v>
@@ -4154,10 +4295,13 @@
       <c r="X47">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:24">
+      <c r="Y47">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B48">
         <v>151.717</v>
@@ -4228,10 +4372,13 @@
       <c r="X48">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:24">
+      <c r="Y48">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25">
       <c r="A49" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B49">
         <v>126.563</v>
@@ -4302,10 +4449,13 @@
       <c r="X49">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:24">
+      <c r="Y49">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25">
       <c r="A50" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B50">
         <v>116.277</v>
@@ -4373,10 +4523,13 @@
       <c r="X50">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:24">
+      <c r="Y50">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25">
       <c r="A51" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B51">
         <v>205.538</v>
@@ -4447,10 +4600,13 @@
       <c r="X51">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:24">
+      <c r="Y51">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
       <c r="A52" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B52">
         <v>122.076</v>
@@ -4521,10 +4677,13 @@
       <c r="X52">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="53" spans="1:24">
+      <c r="Y52">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
       <c r="A53" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B53">
         <v>145.959</v>
@@ -4595,10 +4754,13 @@
       <c r="X53">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="54" spans="1:24">
+      <c r="Y53">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
       <c r="A54" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B54">
         <v>146.286</v>
@@ -4666,10 +4828,13 @@
       <c r="X54">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:24">
+      <c r="Y54">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25">
       <c r="A55" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B55">
         <v>136.889</v>
@@ -4740,10 +4905,13 @@
       <c r="X55">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:24">
+      <c r="Y55">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25">
       <c r="A56" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B56">
         <v>137.606</v>
@@ -4814,10 +4982,13 @@
       <c r="X56">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:24">
+      <c r="Y56">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25">
       <c r="A57" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B57">
         <v>169.592</v>
@@ -4888,10 +5059,13 @@
       <c r="X57">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:24">
+      <c r="Y57">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25">
       <c r="A58" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B58">
         <v>214.169</v>
@@ -4962,10 +5136,13 @@
       <c r="X58">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:24">
+      <c r="Y58">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25">
       <c r="A59" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B59">
         <v>166.109</v>
@@ -5036,10 +5213,13 @@
       <c r="X59">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:24">
+      <c r="Y59">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25">
       <c r="A60" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B60">
         <v>142.899</v>
@@ -5110,10 +5290,13 @@
       <c r="X60">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:24">
+      <c r="Y60">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25">
       <c r="A61" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B61">
         <v>132.64</v>
@@ -5184,10 +5367,13 @@
       <c r="X61">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:24">
+      <c r="Y61">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
       <c r="A62" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B62">
         <v>235.621</v>
@@ -5258,10 +5444,13 @@
       <c r="X62">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:24">
+      <c r="Y62">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25">
       <c r="A63" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B63">
         <v>182.388</v>
@@ -5332,10 +5521,13 @@
       <c r="X63">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:24">
+      <c r="Y63">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25">
       <c r="A64" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B64">
         <v>179.092</v>
@@ -5406,10 +5598,13 @@
       <c r="X64">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:24">
+      <c r="Y64">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25">
       <c r="A65" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B65">
         <v>199.391</v>
@@ -5480,10 +5675,13 @@
       <c r="X65">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="66" spans="1:24">
+      <c r="Y65">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25">
       <c r="A66" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B66">
         <v>294.404</v>
@@ -5554,10 +5752,13 @@
       <c r="X66">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="67" spans="1:24">
+      <c r="Y66">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25">
       <c r="A67" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B67">
         <v>121.06</v>
@@ -5628,10 +5829,13 @@
       <c r="X67">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:24">
+      <c r="Y67">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25">
       <c r="A68" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B68">
         <v>134.968</v>
@@ -5702,10 +5906,13 @@
       <c r="X68">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="69" spans="1:24">
+      <c r="Y68">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25">
       <c r="A69" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B69">
         <v>107.685</v>
@@ -5776,10 +5983,13 @@
       <c r="X69">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="70" spans="1:24">
+      <c r="Y69">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25">
       <c r="A70" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B70">
         <v>106.487</v>
@@ -5847,10 +6057,13 @@
       <c r="X70">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:24">
+      <c r="Y70">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25">
       <c r="A71" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B71">
         <v>142.671</v>
@@ -5921,10 +6134,13 @@
       <c r="X71">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="72" spans="1:24">
+      <c r="Y71">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25">
       <c r="A72" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B72">
         <v>191.36</v>
@@ -5995,10 +6211,13 @@
       <c r="X72">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:24">
+      <c r="Y72">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25">
       <c r="A73" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B73">
         <v>141.614</v>
@@ -6069,10 +6288,13 @@
       <c r="X73">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="74" spans="1:24">
+      <c r="Y73">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25">
       <c r="A74" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B74">
         <v>113.736</v>
@@ -6143,10 +6365,13 @@
       <c r="X74">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:24">
+      <c r="Y74">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25">
       <c r="A75" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B75">
         <v>109.666</v>
@@ -6217,10 +6442,13 @@
       <c r="X75">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:24">
+      <c r="Y75">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25">
       <c r="A76" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B76">
         <v>139.481</v>
@@ -6291,10 +6519,13 @@
       <c r="X76">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:24">
+      <c r="Y76">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25">
       <c r="A77" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B77">
         <v>141.879</v>
@@ -6362,10 +6593,13 @@
       <c r="X77">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:24">
+      <c r="Y77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25">
       <c r="A78" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B78">
         <v>190.392</v>
@@ -6436,10 +6670,13 @@
       <c r="X78">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:24">
+      <c r="Y78">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25">
       <c r="A79" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B79">
         <v>123.225</v>
@@ -6510,10 +6747,13 @@
       <c r="X79">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:24">
+      <c r="Y79">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25">
       <c r="A80" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B80">
         <v>200.64</v>
@@ -6584,10 +6824,13 @@
       <c r="X80">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="81" spans="1:24">
+      <c r="Y80">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25">
       <c r="A81" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B81">
         <v>110.122</v>
@@ -6658,10 +6901,13 @@
       <c r="X81">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:24">
+      <c r="Y81">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25">
       <c r="A82" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B82">
         <v>168.131</v>
@@ -6732,10 +6978,13 @@
       <c r="X82">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="83" spans="1:24">
+      <c r="Y82">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25">
       <c r="A83" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B83">
         <v>128.98</v>
@@ -6805,6 +7054,9 @@
       </c>
       <c r="X83">
         <v>1.5</v>
+      </c>
+      <c r="Y83">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>